<commit_message>
Add output data for debug
</commit_message>
<xml_diff>
--- a/output/demo_2.xlsx
+++ b/output/demo_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\OCR_Nom\experiments\insert_img\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677FD153-BD7C-4FC8-B5A4-25202F91477C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9370F-3CE6-4C71-81D7-48E3DD7F631F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>1_crop_0.jpg</t>
   </si>
   <si>
-    <t>敕大乾國家南海含弘光大至德四位上</t>
-  </si>
-  <si>
     <t>0001</t>
   </si>
   <si>
@@ -61,18 +58,12 @@
     <t>1_crop_2.jpg</t>
   </si>
   <si>
-    <t>壹年值我</t>
-  </si>
-  <si>
     <t>0003</t>
   </si>
   <si>
     <t>1_crop_3.jpg</t>
   </si>
   <si>
-    <t>聖祖仁皇帝五旬大慶節欽奉</t>
-  </si>
-  <si>
     <t>0004</t>
   </si>
   <si>
@@ -80,6 +71,15 @@
   </si>
   <si>
     <t>寶詔潭恩禮隆登秩肆今丕膺</t>
+  </si>
+  <si>
+    <t>值我</t>
+  </si>
+  <si>
+    <t>聖祖仁旬大慶節欽奉</t>
+  </si>
+  <si>
+    <t>敕大乾海含弘至德四位上</t>
   </si>
 </sst>
 </file>
@@ -831,59 +831,59 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="290.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add code to scale image
</commit_message>
<xml_diff>
--- a/output/demo_2.xlsx
+++ b/output/demo_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\OCR_Nom\experiments\insert_img\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9370F-3CE6-4C71-81D7-48E3DD7F631F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CBFF1C-27AF-46CD-A13B-94768A68AFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,15 +49,15 @@
     <t>1_crop_1.jpg</t>
   </si>
   <si>
-    <t>等神護國庇民稔著靈應明命貳拾</t>
-  </si>
-  <si>
     <t>0002</t>
   </si>
   <si>
     <t>1_crop_2.jpg</t>
   </si>
   <si>
+    <t>壹年值我</t>
+  </si>
+  <si>
     <t>0003</t>
   </si>
   <si>
@@ -70,16 +70,16 @@
     <t>1_crop_4.jpg</t>
   </si>
   <si>
-    <t>寶詔潭恩禮隆登秩肆今丕膺</t>
-  </si>
-  <si>
-    <t>值我</t>
-  </si>
-  <si>
-    <t>聖祖仁旬大慶節欽奉</t>
-  </si>
-  <si>
-    <t>敕大乾海含弘至德四位上</t>
+    <t>等神護國著靈應明命貳拾</t>
+  </si>
+  <si>
+    <t>聖祖仁皇帝大慶節欽奉</t>
+  </si>
+  <si>
+    <t>潭恩禮秩肆今丕膺</t>
+  </si>
+  <si>
+    <t>敕大南海含弘光大至德四位上</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="971550" cy="10306050"/>
+    <xdr:ext cx="447675" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1" descr="Picture">
@@ -212,7 +212,7 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="971550" cy="10306050"/>
+    <xdr:ext cx="447675" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Image 2" descr="Picture">
@@ -245,7 +245,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="885825" cy="9648825"/>
+    <xdr:ext cx="428625" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Image 3" descr="Picture">
@@ -278,7 +278,7 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="885825" cy="9648825"/>
+    <xdr:ext cx="428625" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Image 4" descr="Picture">
@@ -311,7 +311,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="762000" cy="2762250"/>
+    <xdr:ext cx="1304925" cy="4752975"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="Image 5" descr="Picture">
@@ -344,7 +344,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="762000" cy="2762250"/>
+    <xdr:ext cx="1304925" cy="4752975"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="Image 6" descr="Picture">
@@ -377,7 +377,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="781050" cy="8172450"/>
+    <xdr:ext cx="447675" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="Image 7" descr="Picture">
@@ -410,7 +410,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="781050" cy="8172450"/>
+    <xdr:ext cx="447675" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="Image 8" descr="Picture">
@@ -443,7 +443,7 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="695325" cy="8191500"/>
+    <xdr:ext cx="400050" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="Image 9" descr="Picture">
@@ -476,7 +476,7 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="695325" cy="8191500"/>
+    <xdr:ext cx="400050" cy="4762500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="11" name="Image 10" descr="Picture">
@@ -844,20 +844,20 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="290.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,7 +870,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>